<commit_message>
Resolve product and customer bug
</commit_message>
<xml_diff>
--- a/data/raw/Country_Master_202406.xlsx
+++ b/data/raw/Country_Master_202406.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28007"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,23 @@
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -7723,9 +7739,9 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -21126,6 +21142,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007CC0BF0D21EA5F4FAAD5CD93A8C42075" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d6a4ca2325726645b16fac471e7daf10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="38b1141c-dc4a-4330-9c18-2e68ed9f285d" xmlns:ns3="7102b333-7a76-4457-b071-5956ef12eb09" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f00ef2c1a799f39092d6c7450fc50714" ns2:_="" ns3:_="">
     <xsd:import namespace="38b1141c-dc4a-4330-9c18-2e68ed9f285d"/>
@@ -21354,38 +21379,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A42B8F-CF14-4F9E-9205-F92279CB13A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="38b1141c-dc4a-4330-9c18-2e68ed9f285d"/>
-    <ds:schemaRef ds:uri="7102b333-7a76-4457-b071-5956ef12eb09"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44DD8895-7B48-44CA-9ACA-E8775DA66729}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44DD8895-7B48-44CA-9ACA-E8775DA66729}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A42B8F-CF14-4F9E-9205-F92279CB13A1}"/>
 </file>
</xml_diff>